<commit_message>
devellopement de la carte slave
</commit_message>
<xml_diff>
--- a/Documentation/Taches.xlsx
+++ b/Documentation/Taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\florian\Desktop\PTC_src\PTC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{198E0E16-B817-47EB-B982-74D363F546FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE756B2-D6E3-4ACD-936A-6B8760042FB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40725" yWindow="3930" windowWidth="21600" windowHeight="15435" xr2:uid="{A7ACE428-3831-4E49-9A8B-418C4775E8D4}"/>
+    <workbookView xWindow="6435" yWindow="2760" windowWidth="21600" windowHeight="15435" xr2:uid="{A7ACE428-3831-4E49-9A8B-418C4775E8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t xml:space="preserve">Fonction </t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Flo</t>
   </si>
 </sst>
 </file>
@@ -300,7 +306,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -356,16 +362,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -692,7 +688,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +832,9 @@
       <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -851,7 +849,9 @@
       <c r="C8" s="4">
         <v>2</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -866,7 +866,9 @@
       <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -896,7 +898,9 @@
       <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -911,7 +915,9 @@
       <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -956,7 +962,9 @@
       <c r="C15" s="4">
         <v>2</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1177,7 +1185,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G3:G4 G6:G29">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",G3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
PWM et Fonction lumiere valide
</commit_message>
<xml_diff>
--- a/Documentation/Taches.xlsx
+++ b/Documentation/Taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\florian\Desktop\PTC_src\PTC\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Bureau\FLORIAN\PTC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE756B2-D6E3-4ACD-936A-6B8760042FB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF512DC-A660-412F-8D4B-3A91530278FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6435" yWindow="2760" windowWidth="21600" windowHeight="15435" xr2:uid="{A7ACE428-3831-4E49-9A8B-418C4775E8D4}"/>
+    <workbookView xWindow="855" yWindow="1485" windowWidth="14625" windowHeight="13860" xr2:uid="{A7ACE428-3831-4E49-9A8B-418C4775E8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t xml:space="preserve">Fonction </t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>Flo</t>
+  </si>
+  <si>
+    <t>Points</t>
   </si>
 </sst>
 </file>
@@ -287,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -302,6 +305,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D48D154-4584-4323-9E05-9BBB0E5EA430}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +704,7 @@
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -722,8 +726,11 @@
       <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -745,8 +752,11 @@
       <c r="G2" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -760,8 +770,11 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -783,8 +796,11 @@
       <c r="G4" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -806,8 +822,11 @@
       <c r="G5" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -817,12 +836,19 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H6" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -838,8 +864,11 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -855,8 +884,11 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -872,8 +904,11 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -883,12 +918,17 @@
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -904,8 +944,11 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -921,8 +964,11 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -936,8 +982,11 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -951,8 +1000,11 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -968,8 +1020,11 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -983,8 +1038,11 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -998,8 +1056,11 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1013,8 +1074,11 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1028,8 +1092,11 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1043,8 +1110,11 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1058,8 +1128,11 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1073,8 +1146,11 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1088,8 +1164,11 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1103,8 +1182,11 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1118,8 +1200,11 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1133,8 +1218,11 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1148,8 +1236,11 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1163,8 +1254,11 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1178,8 +1272,11 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>

</xml_diff>

<commit_message>
ajout de fonction de detection de commande
</commit_message>
<xml_diff>
--- a/Documentation/Taches.xlsx
+++ b/Documentation/Taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Bureau\FLORIAN\PTC\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF512DC-A660-412F-8D4B-3A91530278FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC13B957-8819-49E0-9253-721F640AE168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="1485" windowWidth="14625" windowHeight="13860" xr2:uid="{A7ACE428-3831-4E49-9A8B-418C4775E8D4}"/>
+    <workbookView xWindow="855" yWindow="1485" windowWidth="19335" windowHeight="13860" xr2:uid="{A7ACE428-3831-4E49-9A8B-418C4775E8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D48D154-4584-4323-9E05-9BBB0E5EA430}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,22 +1301,22 @@
       <formula>NOT(ISERROR(SEARCH("NO",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E4 E6:E29">
+  <conditionalFormatting sqref="E3:E4 E6:E29 F10">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E4 E6:E29">
+  <conditionalFormatting sqref="E3:E4 E6:E29 F10">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F4 F6:F29">
+  <conditionalFormatting sqref="F3:F4 F6:F9 F11:F29">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F4 F6:F29">
+  <conditionalFormatting sqref="F3:F4 F6:F9 F11:F29">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",F3)))</formula>
     </cfRule>

</xml_diff>